<commit_message>
update R1, R2, R3 to 100ohm
</commit_message>
<xml_diff>
--- a/Doc/PartsList.xlsx
+++ b/Doc/PartsList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d02517ffe0afae64/make/_K-0025_Si4735Radio/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="394" documentId="11_AD4D066CA252ABDACC1048C2A1D3D80C72EEDF56" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4A3F9DF-D574-49B0-A57B-85D747215138}"/>
+  <xr:revisionPtr revIDLastSave="417" documentId="11_AD4D066CA252ABDACC1048C2A1D3D80C72EEDF56" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41A9311D-BF14-4FF5-AAA5-9FA24AD07A84}"/>
   <bookViews>
-    <workbookView xWindow="5625" yWindow="960" windowWidth="28320" windowHeight="18465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10785" yWindow="600" windowWidth="23925" windowHeight="18465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="220">
   <si>
     <t>Qty</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>R1, R2</t>
-  </si>
-  <si>
-    <t>R3, R4, R5, R6</t>
   </si>
   <si>
     <t>541-3951-1-ND</t>
@@ -323,26 +320,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>541-5512-1-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.jp/ja/products/detail/vishay-dale/CRCW0603620RFKEAC/7924102</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>R2, R3</t>
-  </si>
-  <si>
-    <t>541-3953-1-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.jp/ja/products/detail/vishay-dale/CRCW06032K00FKEAC/7928375</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>R4</t>
   </si>
   <si>
@@ -638,14 +615,6 @@
   </si>
   <si>
     <t>FT37-77 (5977000201) 12T</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>600 SMD 0603(1608)</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>2k SMD 0603(1608)</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -806,21 +775,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">J2, J3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>**1</t>
-    </r>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>1x2 Pin Header</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -841,21 +795,6 @@
   </si>
   <si>
     <t>Pin Header 1x40 R/A</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">J1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>**1</t>
-    </r>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -930,11 +869,76 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
+    <t>**2</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1uF (100n) </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">C1 </t>
+      <t xml:space="preserve">R1, R2, R3 </t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>**3</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">R3, R4, R5, R6 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>**3</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>**3</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>100 ohm</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">J1 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>**1</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C2, C12, C16 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Consolas"/>
@@ -946,10 +950,27 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">C2, C12, C16 </t>
+      <t xml:space="preserve">J2, J3 </t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>**1</t>
+    </r>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C1 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Consolas"/>
@@ -960,11 +981,7 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>**2</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1uF (100n) </t>
+    <t>100 SMD 0603(1608)</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1350,7 +1367,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1509,6 +1526,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1797,10 +1823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F72"/>
+  <dimension ref="B2:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1816,7 +1842,7 @@
   <sheetData>
     <row r="2" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
       <c r="B2" s="1" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
@@ -1830,27 +1856,27 @@
         <v>2</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickTop="1">
       <c r="B4" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="12">
+        <v>1</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="12">
-        <v>1</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="25" t="s">
         <v>19</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
@@ -1878,7 +1904,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>4</v>
@@ -1889,13 +1915,13 @@
     </row>
     <row r="7" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B7" s="14" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="C7" s="8">
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="53"/>
@@ -1908,77 +1934,73 @@
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B9" s="14" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="C9" s="8">
         <v>4</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>13</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="53"/>
     </row>
     <row r="10" spans="2:6" s="1" customFormat="1" ht="25.5">
       <c r="B10" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="8">
         <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="2:6" s="1" customFormat="1">
       <c r="B11" s="27" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C11" s="11">
         <v>1</v>
       </c>
       <c r="D11" s="61" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="53"/>
     </row>
     <row r="12" spans="2:6" s="1" customFormat="1">
       <c r="B12" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="11">
         <v>2</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="18" t="s">
         <v>16</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:6" s="1" customFormat="1" ht="13.5" thickBot="1">
@@ -1986,10 +2008,10 @@
       <c r="C13" s="20"/>
       <c r="D13" s="21"/>
       <c r="E13" s="22" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
@@ -1997,7 +2019,7 @@
     </row>
     <row r="15" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
       <c r="B15" s="1" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
@@ -2015,844 +2037,845 @@
     </row>
     <row r="17" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickTop="1">
       <c r="B17" s="28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="12">
         <v>1</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E17" s="33" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F17" s="38" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B18" s="16" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C18" s="8">
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B19" s="16" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C19" s="8">
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="F19" s="29" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B20" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="8">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="8">
-        <v>1</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E20" s="3" t="s">
+      <c r="F20" s="29" t="s">
         <v>83</v>
-      </c>
-      <c r="F20" s="29" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="21" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B21" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="8">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="8">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E21" s="3" t="s">
+      <c r="F21" s="29" t="s">
         <v>22</v>
-      </c>
-      <c r="F21" s="29" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="22" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B22" s="16" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C22" s="8">
         <v>3</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="54"/>
     </row>
     <row r="23" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B23" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="8">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="8">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="F23" s="29" t="s">
         <v>27</v>
-      </c>
-      <c r="F23" s="29" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="24" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B24" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="8">
         <v>2</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="F24" s="29" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="25" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B25" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="8">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="8">
-        <v>1</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="F25" s="29" t="s">
         <v>33</v>
-      </c>
-      <c r="F25" s="29" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="26" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B26" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="8">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="8">
-        <v>1</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" s="29" t="s">
         <v>36</v>
-      </c>
-      <c r="F26" s="29" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="27" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B27" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C27" s="8">
         <v>2</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="29" t="s">
         <v>42</v>
-      </c>
-      <c r="F27" s="29" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="28" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B28" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C28" s="8">
         <v>3</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="29" t="s">
         <v>45</v>
-      </c>
-      <c r="F28" s="29" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="29" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B29" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C29" s="8">
         <v>4</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E29" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="29" t="s">
         <v>48</v>
-      </c>
-      <c r="F29" s="29" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="30" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B30" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" s="8">
         <v>2</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="E30" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="29" t="s">
         <v>51</v>
-      </c>
-      <c r="F30" s="29" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="31" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B31" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="8">
+        <v>1</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="8">
-        <v>1</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="29" t="s">
         <v>54</v>
-      </c>
-      <c r="F31" s="29" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="32" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B32" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="8">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="8">
-        <v>1</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E32" s="3" t="s">
+      <c r="F32" s="29" t="s">
         <v>57</v>
-      </c>
-      <c r="F32" s="29" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="33" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B33" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C33" s="8">
         <v>6</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="E33" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" s="29" t="s">
         <v>60</v>
-      </c>
-      <c r="F33" s="29" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="34" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B34" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C34" s="8">
         <v>5</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E34" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" s="29" t="s">
         <v>63</v>
-      </c>
-      <c r="F34" s="29" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="35" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B35" s="16" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C35" s="8">
         <v>1</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="54"/>
     </row>
     <row r="36" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B36" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="8">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="8">
-        <v>1</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E36" s="3" t="s">
+      <c r="F36" s="29" t="s">
         <v>66</v>
-      </c>
-      <c r="F36" s="29" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="37" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B37" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="8">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="8">
-        <v>1</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E37" s="2" t="s">
+      <c r="F37" s="29" t="s">
         <v>69</v>
-      </c>
-      <c r="F37" s="29" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="38" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B38" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C38" s="8">
         <v>2</v>
       </c>
       <c r="D38" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="F38" s="29" t="s">
         <v>73</v>
-      </c>
-      <c r="F38" s="29" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="39" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B39" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="8">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="8">
-        <v>1</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E39" s="3" t="s">
+      <c r="F39" s="29" t="s">
         <v>76</v>
-      </c>
-      <c r="F39" s="29" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="40" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B40" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="8">
+        <v>1</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="8">
-        <v>1</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E40" s="3" t="s">
+      <c r="F40" s="29" t="s">
         <v>79</v>
-      </c>
-      <c r="F40" s="29" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="41" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B41" s="16" t="s">
-        <v>85</v>
+        <v>211</v>
       </c>
       <c r="C41" s="8">
-        <v>1</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F41" s="29" t="s">
-        <v>87</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E41" s="6"/>
+      <c r="F41" s="53"/>
     </row>
     <row r="42" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B42" s="16" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C42" s="8">
-        <v>2</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>174</v>
+        <v>1</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>166</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F42" s="29" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B43" s="16" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C43" s="8">
         <v>1</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>175</v>
+      <c r="D43" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F43" s="29" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B44" s="16" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C44" s="8">
         <v>1</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F44" s="29" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B45" s="16" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C45" s="8">
         <v>1</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F45" s="29" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B46" s="16" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C46" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F46" s="29" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B47" s="16" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C47" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F47" s="29" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B48" s="16" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C48" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F48" s="29" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B49" s="16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C49" s="8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F49" s="29" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B50" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C50" s="8">
         <v>2</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="E50" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F50" s="29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
+      <c r="B51" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" s="11">
+        <v>1</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F51" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="F50" s="29" t="s">
+    </row>
+    <row r="52" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
+      <c r="B52" s="28"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="F52" s="29" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
+      <c r="B53" s="16" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="51" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
-      <c r="B51" s="16" t="s">
+      <c r="C53" s="8">
+        <v>1</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C51" s="8">
-        <v>2</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="E51" s="3" t="s">
+      <c r="F53" s="29" t="s">
         <v>117</v>
-      </c>
-      <c r="F51" s="29" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
-      <c r="B52" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="C52" s="11">
-        <v>1</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F52" s="29" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
-      <c r="B53" s="28"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="F53" s="29" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="54" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
       <c r="B54" s="16" t="s">
-        <v>122</v>
+        <v>202</v>
       </c>
       <c r="C54" s="8">
         <v>1</v>
       </c>
       <c r="D54" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E54" s="48"/>
+      <c r="F54" s="29"/>
+    </row>
+    <row r="55" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
+      <c r="B55" s="44" t="s">
+        <v>197</v>
+      </c>
+      <c r="C55" s="20">
+        <v>1</v>
+      </c>
+      <c r="D55" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="E55" s="46" t="s">
+        <v>181</v>
+      </c>
+      <c r="F55" s="47" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1"/>
+    <row r="57" spans="2:6" s="1" customFormat="1" ht="15" thickBot="1">
+      <c r="B57" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
+      <c r="B58" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E58" s="36"/>
+      <c r="F58" s="37"/>
+    </row>
+    <row r="59" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickTop="1">
+      <c r="B59" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="C59" s="12">
+        <v>1</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="E59" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="F59" s="38" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
+      <c r="B60" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C60" s="31">
+        <v>2</v>
+      </c>
+      <c r="D60" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="E60" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F60" s="39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" s="1" customFormat="1"/>
+    <row r="62" spans="2:6" s="1" customFormat="1" ht="15" thickBot="1">
+      <c r="B62" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
+      <c r="B63" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E63" s="36"/>
+      <c r="F63" s="37"/>
+    </row>
+    <row r="64" spans="2:6" s="1" customFormat="1" ht="13.5" thickTop="1">
+      <c r="B64" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="C64" s="12">
+        <v>8</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="F64" s="43" t="s">
         <v>184</v>
       </c>
-      <c r="E54" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="F54" s="29" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1">
-      <c r="B55" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="C55" s="8">
-        <v>1</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="E55" s="48"/>
-      <c r="F55" s="29"/>
-    </row>
-    <row r="56" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="B56" s="44" t="s">
-        <v>206</v>
-      </c>
-      <c r="C56" s="20">
-        <v>1</v>
-      </c>
-      <c r="D56" s="21" t="s">
-        <v>205</v>
-      </c>
-      <c r="E56" s="46" t="s">
-        <v>190</v>
-      </c>
-      <c r="F56" s="47" t="s">
+    </row>
+    <row r="65" spans="2:6">
+      <c r="B65" s="42" t="s">
+        <v>194</v>
+      </c>
+      <c r="C65" s="60">
+        <v>8</v>
+      </c>
+      <c r="D65" s="40" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="57" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1"/>
-    <row r="58" spans="2:6" s="1" customFormat="1" ht="15" thickBot="1">
-      <c r="B58" s="1" t="s">
+      <c r="E65" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="F65" s="41" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="B59" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="C59" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="D59" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="E59" s="36"/>
-      <c r="F59" s="37"/>
-    </row>
-    <row r="60" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickTop="1">
-      <c r="B60" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="C60" s="12">
-        <v>1</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="E60" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="F60" s="38" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="B61" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="C61" s="31">
-        <v>2</v>
-      </c>
-      <c r="D61" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="E61" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="F61" s="39" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" s="1" customFormat="1"/>
-    <row r="63" spans="2:6" s="1" customFormat="1" ht="15" thickBot="1">
-      <c r="B63" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="B64" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="C64" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="D64" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="E64" s="36"/>
-      <c r="F64" s="37"/>
-    </row>
-    <row r="65" spans="2:6" s="1" customFormat="1" ht="13.5" thickTop="1">
-      <c r="B65" s="24" t="s">
-        <v>202</v>
-      </c>
-      <c r="C65" s="12">
-        <v>8</v>
-      </c>
-      <c r="D65" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="E65" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="F65" s="43" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="66" spans="2:6">
       <c r="B66" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="C66" s="60">
+        <v>4</v>
+      </c>
+      <c r="D66" s="40" t="s">
+        <v>195</v>
+      </c>
+      <c r="E66" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="F66" s="41" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B67" s="55" t="s">
+        <v>207</v>
+      </c>
+      <c r="C67" s="56">
+        <v>1</v>
+      </c>
+      <c r="D67" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="E67" s="58"/>
+      <c r="F67" s="59"/>
+    </row>
+    <row r="68" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B68" s="45" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
+      <c r="B69" s="49" t="s">
         <v>203</v>
       </c>
-      <c r="C66" s="60">
-        <v>8</v>
-      </c>
-      <c r="D66" s="40" t="s">
+      <c r="C69" s="50">
+        <v>1</v>
+      </c>
+      <c r="D69" s="51" t="s">
         <v>198</v>
       </c>
-      <c r="E66" s="40" t="s">
-        <v>196</v>
-      </c>
-      <c r="F66" s="41" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6">
-      <c r="B67" s="42" t="s">
-        <v>201</v>
-      </c>
-      <c r="C67" s="60">
-        <v>4</v>
-      </c>
-      <c r="D67" s="40" t="s">
-        <v>204</v>
-      </c>
-      <c r="E67" s="40" t="s">
-        <v>200</v>
-      </c>
-      <c r="F67" s="41" t="s">
+      <c r="E69" s="51" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="68" spans="2:6" ht="13.5" thickBot="1">
-      <c r="B68" s="55" t="s">
-        <v>218</v>
-      </c>
-      <c r="C68" s="56">
-        <v>1</v>
-      </c>
-      <c r="D68" s="57" t="s">
-        <v>219</v>
-      </c>
-      <c r="E68" s="58"/>
-      <c r="F68" s="59"/>
-    </row>
-    <row r="69" spans="2:6" ht="13.5" thickBot="1">
-      <c r="B69" s="45" t="s">
+      <c r="F69" s="52" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B70" s="45" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="70" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="B70" s="49" t="s">
+    <row r="71" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
+      <c r="B71" s="49" t="s">
+        <v>210</v>
+      </c>
+      <c r="C71" s="50">
+        <v>3</v>
+      </c>
+      <c r="D71" s="51" t="s">
+        <v>145</v>
+      </c>
+      <c r="E71" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="F71" s="52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B72" s="45" t="s">
         <v>213</v>
       </c>
-      <c r="C70" s="50">
-        <v>1</v>
-      </c>
-      <c r="D70" s="51" t="s">
-        <v>207</v>
-      </c>
-      <c r="E70" s="51" t="s">
-        <v>208</v>
-      </c>
-      <c r="F70" s="52" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" ht="13.5" thickBot="1">
-      <c r="B71" s="45" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="72" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
-      <c r="B72" s="49" t="s">
-        <v>223</v>
-      </c>
-      <c r="C72" s="50">
-        <v>3</v>
-      </c>
-      <c r="D72" s="51" t="s">
-        <v>152</v>
-      </c>
-      <c r="E72" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="F72" s="52" t="s">
-        <v>25</v>
+    </row>
+    <row r="73" spans="2:6" s="1" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
+      <c r="B73" s="62" t="s">
+        <v>214</v>
+      </c>
+      <c r="C73" s="50">
+        <v>7</v>
+      </c>
+      <c r="D73" s="63" t="s">
+        <v>137</v>
+      </c>
+      <c r="E73" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F73" s="64" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2863,7 +2886,7 @@
     <hyperlink ref="F17" r:id="rId3" xr:uid="{7FF0D5C2-46F5-472A-A828-B85EB718CBD2}"/>
     <hyperlink ref="F18" r:id="rId4" xr:uid="{A503D196-36D0-4751-94F8-9C9CAA743C87}"/>
     <hyperlink ref="F19" r:id="rId5" xr:uid="{C68628E2-1C02-430D-B1D7-97550FC84A4D}"/>
-    <hyperlink ref="F52" r:id="rId6" xr:uid="{D9BA017C-AD0C-4C4E-A0DA-54F0706E4050}"/>
+    <hyperlink ref="F51" r:id="rId6" xr:uid="{D9BA017C-AD0C-4C4E-A0DA-54F0706E4050}"/>
     <hyperlink ref="F40" r:id="rId7" xr:uid="{B3B0D1D8-3AD7-4893-B146-FB52EB81C10A}"/>
     <hyperlink ref="F32" r:id="rId8" xr:uid="{67A6EBE0-87F8-4DA0-AB3A-CFF3456CCF20}"/>
     <hyperlink ref="F34" r:id="rId9" xr:uid="{E50E767A-313D-4A0D-9F2B-E457B7EF74F8}"/>
@@ -2878,39 +2901,37 @@
     <hyperlink ref="F5" r:id="rId18" xr:uid="{2F2E2BFC-A011-4943-93C1-063370B2A915}"/>
     <hyperlink ref="F23" r:id="rId19" xr:uid="{1E9B64AE-0A13-485E-9294-02E13AC2CDFD}"/>
     <hyperlink ref="F25" r:id="rId20" xr:uid="{1AAEB439-7E62-4211-8EB6-70A0FA78B821}"/>
-    <hyperlink ref="F61" r:id="rId21" xr:uid="{6A2BA7DE-B2D3-4A1F-8980-CFFE57010C82}"/>
+    <hyperlink ref="F60" r:id="rId21" xr:uid="{6A2BA7DE-B2D3-4A1F-8980-CFFE57010C82}"/>
     <hyperlink ref="F28" r:id="rId22" xr:uid="{06DDCC70-ECA4-492C-BA99-9DB6B4F82941}"/>
     <hyperlink ref="F29" r:id="rId23" xr:uid="{800E211D-E6F5-4173-9C8A-4B1A2A330F03}"/>
     <hyperlink ref="F31" r:id="rId24" xr:uid="{2A6B2FD4-B290-444A-B3C5-3488017A06E6}"/>
     <hyperlink ref="F33" r:id="rId25" xr:uid="{61C16AB5-F17A-42C8-B961-49B86A29CAEA}"/>
     <hyperlink ref="F20" r:id="rId26" xr:uid="{4A3EA232-6657-46F1-9732-95D61C89E09A}"/>
-    <hyperlink ref="F41" r:id="rId27" xr:uid="{A5F50DE1-786E-4903-8E42-F06710F2F373}"/>
-    <hyperlink ref="F43" r:id="rId28" xr:uid="{0B7B93B4-95F4-4329-BD7D-BA70D753001E}"/>
-    <hyperlink ref="F44" r:id="rId29" xr:uid="{6F63D64E-E633-4B43-B0AD-B977C311DBDE}"/>
-    <hyperlink ref="F45" r:id="rId30" xr:uid="{09055E1D-C0D9-4552-B7C6-85DA2261252B}"/>
-    <hyperlink ref="F47" r:id="rId31" xr:uid="{78D07AE9-5E10-475D-A348-9D2643F8424F}"/>
-    <hyperlink ref="F48" r:id="rId32" xr:uid="{72356A6F-498C-4F5F-8130-2F180F05A899}"/>
-    <hyperlink ref="F49" r:id="rId33" xr:uid="{9F9DEBA3-F6C3-4095-A85A-FC5CAC7BF5B2}"/>
-    <hyperlink ref="F50" r:id="rId34" xr:uid="{32120286-892A-4AB9-B6A6-B8A66C730E94}"/>
-    <hyperlink ref="F51" r:id="rId35" xr:uid="{9E935C90-02CE-4AC6-959C-7F3E704C0134}"/>
-    <hyperlink ref="F54" r:id="rId36" xr:uid="{572796EE-9C85-47A7-879A-7AAF25CE69B2}"/>
-    <hyperlink ref="F60" r:id="rId37" xr:uid="{8C83ABD2-811F-4CBB-AAF6-33B0B387185E}"/>
-    <hyperlink ref="F9" r:id="rId38" xr:uid="{30211986-7769-4149-A873-BDD413A90CB4}"/>
-    <hyperlink ref="F8" r:id="rId39" xr:uid="{E01FDBF2-2137-4ED5-8D4B-7B481BFF8F3D}"/>
-    <hyperlink ref="F46" r:id="rId40" xr:uid="{3CD61206-22CA-4F6C-B479-A45C2FA28ACC}"/>
-    <hyperlink ref="F42" r:id="rId41" xr:uid="{4BC46CB1-FAE8-4269-8196-6C79EC4526CC}"/>
-    <hyperlink ref="F39" r:id="rId42" xr:uid="{5198CAF9-EEF7-472E-8FD9-7F68B0D5F9F2}"/>
-    <hyperlink ref="F36" r:id="rId43" xr:uid="{B58F5F05-EE4A-451B-8A03-132039EC1096}"/>
-    <hyperlink ref="F10" r:id="rId44" xr:uid="{B550A6E1-4D0B-4BC1-BA23-F1BD9EF125E1}"/>
-    <hyperlink ref="F53" r:id="rId45" xr:uid="{B9A79773-4643-4C76-BC28-1E4C476A19C8}"/>
-    <hyperlink ref="F56" r:id="rId46" xr:uid="{61E4FEA9-5A61-46A8-AE7F-1051108F3BD6}"/>
-    <hyperlink ref="F65" r:id="rId47" xr:uid="{91B84E00-3D11-4713-B945-05090D349F83}"/>
-    <hyperlink ref="F66" r:id="rId48" xr:uid="{D9D343BC-D714-48AE-B370-053CB74AB9CA}"/>
-    <hyperlink ref="F67" r:id="rId49" xr:uid="{958EC69A-EBB6-4963-BDDF-120872B119B8}"/>
-    <hyperlink ref="F70" r:id="rId50" xr:uid="{30110872-E5B0-4393-BBB8-E796AC34B717}"/>
-    <hyperlink ref="F72" r:id="rId51" xr:uid="{7B969707-3D4A-4D03-8472-31353B8B1701}"/>
+    <hyperlink ref="F42" r:id="rId27" xr:uid="{0B7B93B4-95F4-4329-BD7D-BA70D753001E}"/>
+    <hyperlink ref="F43" r:id="rId28" xr:uid="{6F63D64E-E633-4B43-B0AD-B977C311DBDE}"/>
+    <hyperlink ref="F44" r:id="rId29" xr:uid="{09055E1D-C0D9-4552-B7C6-85DA2261252B}"/>
+    <hyperlink ref="F46" r:id="rId30" xr:uid="{78D07AE9-5E10-475D-A348-9D2643F8424F}"/>
+    <hyperlink ref="F47" r:id="rId31" xr:uid="{72356A6F-498C-4F5F-8130-2F180F05A899}"/>
+    <hyperlink ref="F48" r:id="rId32" xr:uid="{9F9DEBA3-F6C3-4095-A85A-FC5CAC7BF5B2}"/>
+    <hyperlink ref="F49" r:id="rId33" xr:uid="{32120286-892A-4AB9-B6A6-B8A66C730E94}"/>
+    <hyperlink ref="F50" r:id="rId34" xr:uid="{9E935C90-02CE-4AC6-959C-7F3E704C0134}"/>
+    <hyperlink ref="F53" r:id="rId35" xr:uid="{572796EE-9C85-47A7-879A-7AAF25CE69B2}"/>
+    <hyperlink ref="F59" r:id="rId36" xr:uid="{8C83ABD2-811F-4CBB-AAF6-33B0B387185E}"/>
+    <hyperlink ref="F8" r:id="rId37" xr:uid="{E01FDBF2-2137-4ED5-8D4B-7B481BFF8F3D}"/>
+    <hyperlink ref="F45" r:id="rId38" xr:uid="{3CD61206-22CA-4F6C-B479-A45C2FA28ACC}"/>
+    <hyperlink ref="F39" r:id="rId39" xr:uid="{5198CAF9-EEF7-472E-8FD9-7F68B0D5F9F2}"/>
+    <hyperlink ref="F36" r:id="rId40" xr:uid="{B58F5F05-EE4A-451B-8A03-132039EC1096}"/>
+    <hyperlink ref="F10" r:id="rId41" xr:uid="{B550A6E1-4D0B-4BC1-BA23-F1BD9EF125E1}"/>
+    <hyperlink ref="F52" r:id="rId42" xr:uid="{B9A79773-4643-4C76-BC28-1E4C476A19C8}"/>
+    <hyperlink ref="F55" r:id="rId43" xr:uid="{61E4FEA9-5A61-46A8-AE7F-1051108F3BD6}"/>
+    <hyperlink ref="F64" r:id="rId44" xr:uid="{91B84E00-3D11-4713-B945-05090D349F83}"/>
+    <hyperlink ref="F65" r:id="rId45" xr:uid="{D9D343BC-D714-48AE-B370-053CB74AB9CA}"/>
+    <hyperlink ref="F66" r:id="rId46" xr:uid="{958EC69A-EBB6-4963-BDDF-120872B119B8}"/>
+    <hyperlink ref="F69" r:id="rId47" xr:uid="{30110872-E5B0-4393-BBB8-E796AC34B717}"/>
+    <hyperlink ref="F71" r:id="rId48" xr:uid="{7B969707-3D4A-4D03-8472-31353B8B1701}"/>
+    <hyperlink ref="F73" r:id="rId49" xr:uid="{31C28C1C-F8DE-4C20-A520-C3B37D5B77BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId52"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId50"/>
 </worksheet>
 </file>
</xml_diff>